<commit_message>
day 18 and XML+RMI
</commit_message>
<xml_diff>
--- a/invoice.xlsx
+++ b/invoice.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Description</t>
   </si>
@@ -26,49 +26,22 @@
     <t>Total Price</t>
   </si>
   <si>
-    <t>Web Design</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>1000.0</t>
-  </si>
-  <si>
-    <t>Logo Design</t>
+    <t>daal</t>
   </si>
   <si>
     <t>2</t>
   </si>
   <si>
-    <t>420.0</t>
-  </si>
-  <si>
-    <t>840.0</t>
-  </si>
-  <si>
-    <t>Animation Video</t>
-  </si>
-  <si>
-    <t>399.9</t>
-  </si>
-  <si>
-    <t>Image Editing</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>450.0</t>
-  </si>
-  <si>
-    <t>1350.0</t>
+    <t>12.0</t>
+  </si>
+  <si>
+    <t>24.0</t>
   </si>
   <si>
     <t>SubTotal</t>
   </si>
   <si>
-    <t>3589.90</t>
+    <t>48.00</t>
   </si>
   <si>
     <t>Discount</t>
@@ -80,13 +53,13 @@
     <t>SubTotal Less Discount</t>
   </si>
   <si>
-    <t>3948.89</t>
+    <t>52.80</t>
   </si>
   <si>
     <t>Tax Rate</t>
   </si>
   <si>
-    <t>4146.33</t>
+    <t>55.44</t>
   </si>
   <si>
     <t>Shipping/Handling</t>
@@ -98,7 +71,7 @@
     <t>Balance</t>
   </si>
   <si>
-    <t>4048.89</t>
+    <t>152.80</t>
   </si>
 </sst>
 </file>
@@ -143,13 +116,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.7890625" collapsed="false"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.22265625" collapsed="false"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="4.76953125" collapsed="false"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="21.7265625" collapsed="false"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="10.390625" collapsed="false"/>
@@ -180,97 +153,69 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="4">
+      <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D4" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
+    </row>
+    <row r="5">
+      <c r="C5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
+      <c r="D5" t="s">
         <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="6">
       <c r="C6" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7">
       <c r="C7" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8">
       <c r="C8" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9">
       <c r="C9" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="C10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="C11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>